<commit_message>
Modificaciones en la bitácora
</commit_message>
<xml_diff>
--- a/Bitácora Experiencia 1.xlsx
+++ b/Bitácora Experiencia 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocki\Documents\TERCER SEMESTRE\PROGRAMACIÓN WEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocki\Desktop\Experiencia 1 - Soraya Soto\Experiencia1_SotoSoraya_006D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F2D999-6D73-4888-925A-0F72F282C0CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A31F5E-04D3-4D02-8458-D4C5556A12A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1185" windowWidth="16395" windowHeight="11610" xr2:uid="{666F6319-EEC7-43AC-8618-9CA485670A34}"/>
+    <workbookView xWindow="8490" yWindow="1740" windowWidth="16395" windowHeight="11610" xr2:uid="{666F6319-EEC7-43AC-8618-9CA485670A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Equipo</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Modificaciones en about</t>
+  </si>
+  <si>
+    <t>Ajustes finales página web</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="B2:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,10 +717,18 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="5">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="6">
+        <v>44298</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
@@ -728,7 +739,7 @@
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>